<commit_message>
Work 2019/03/24 Before SpecSyzer
</commit_message>
<xml_diff>
--- a/bin/lib/Astro_Libraries/literature_data/lines_data.xlsx
+++ b/bin/lib/Astro_Libraries/literature_data/lines_data.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vital\PycharmProjects\dazer\bin\lib\Astro_Libraries\literature_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2B47A0-0341-43B7-8C43-55F228EC3942}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="19968" yWindow="2436" windowWidth="14928" windowHeight="14244" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,638 +28,619 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="201">
   <si>
-    <t xml:space="preserve">wavelength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pyneb_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pyneb_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emis_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latex_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_3835A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3835.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3835A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3835$ $H9$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_3726A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3726.032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3726A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3726$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_3726A_b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3727.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3726 + 3729$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_3729A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3728.815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3729</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3729A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3729$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_3889A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3889.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3889</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3889A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3889$ $H8 + HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_3889A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_3970A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3970.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3970</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3970A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$3889$ $H\epsilon$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_4026A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4026.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4026A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4026$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_4102A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4102.742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4102A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4102$ $H\delta$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_4341A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4341.471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4341A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4341$ $H\gamma$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3_4363A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4363.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4363</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4363A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4363$ $[OIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_4471A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4471.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4471A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4471$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar4_4740A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4740A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4470$ $[ArIV]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He2_4686A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4686.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He2r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4686A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4686$ $HeII$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_4861A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4861.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4861</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4861A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4861$ $H\beta$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3_4959A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4958.911</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4959A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$4959$ $[OIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O3_5007A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5006.843</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5007A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5007$ $[OIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2_5755A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5755.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5755A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5755$ $[NII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_5876A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5876.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5876A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5876$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3_6312A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6312.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6312A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6312$ $[SIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2_6548A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6548.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6548</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6548A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6548$ $[NII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_6563A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6562.819</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6563A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6563$ $H\alpha$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2_6584A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6583.46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6584</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6584A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6583$ $[NII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_6678A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6678.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6678A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6678$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S2_6716A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6716.44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6716</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6716A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6717$ $[SII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S2_6731A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6730.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6731A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$6731$ $[SII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_7065A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7065.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7065A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7065$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_7281A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7281.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7281</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7281A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7281$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar3_7136A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7136A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7136$ $[NII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_7319A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7319.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7319A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7319$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7319A+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_7319A_b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7324.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7319 + 7330$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2_7330A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7330.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7330A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7330$ $[OII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7330A+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar3_7751A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7751A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7751$ $[NII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3_9069A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9068.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9069A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$9069$ $[SIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_9229A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9229.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9229A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$9229$ $Hpa9$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3_9531A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9531.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9531A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$9531$ $[SIII]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1_9546A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9546.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9546</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9546A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$9531$ $Hpa9$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1_10830A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10830.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10830</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10830A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$10830$ $HeI$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4102.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4341.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6563.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He1</t>
+    <t>wavelength</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>pyneb_code</t>
+  </si>
+  <si>
+    <t>pyneb_label</t>
+  </si>
+  <si>
+    <t>emis_type</t>
+  </si>
+  <si>
+    <t>latex_code</t>
+  </si>
+  <si>
+    <t>coments</t>
+  </si>
+  <si>
+    <t>H1_3835A</t>
+  </si>
+  <si>
+    <t>3835.0</t>
+  </si>
+  <si>
+    <t>H1r</t>
+  </si>
+  <si>
+    <t>3835</t>
+  </si>
+  <si>
+    <t>3835A</t>
+  </si>
+  <si>
+    <t>rec</t>
+  </si>
+  <si>
+    <t>$3835$ $H9$</t>
+  </si>
+  <si>
+    <t>O2_3726A</t>
+  </si>
+  <si>
+    <t>3726.032</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>3726</t>
+  </si>
+  <si>
+    <t>3726A</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>$3726$ $[OII]$</t>
+  </si>
+  <si>
+    <t>O2_3726A_b</t>
+  </si>
+  <si>
+    <t>3727.5</t>
+  </si>
+  <si>
+    <t>$3726 + 3729$ $[OII]$</t>
+  </si>
+  <si>
+    <t>O2_3729A</t>
+  </si>
+  <si>
+    <t>3728.815</t>
+  </si>
+  <si>
+    <t>3729</t>
+  </si>
+  <si>
+    <t>3729A</t>
+  </si>
+  <si>
+    <t>$3729$ $[OII]$</t>
+  </si>
+  <si>
+    <t>H1_3889A</t>
+  </si>
+  <si>
+    <t>3889.0</t>
+  </si>
+  <si>
+    <t>3889</t>
+  </si>
+  <si>
+    <t>3889A</t>
+  </si>
+  <si>
+    <t>$3889$ $H8 + HeI$</t>
+  </si>
+  <si>
+    <t>He1_3889A</t>
+  </si>
+  <si>
+    <t>He1r</t>
+  </si>
+  <si>
+    <t>H1_3970A</t>
+  </si>
+  <si>
+    <t>3970.0</t>
+  </si>
+  <si>
+    <t>3970</t>
+  </si>
+  <si>
+    <t>3970A</t>
+  </si>
+  <si>
+    <t>$3889$ $H\epsilon$</t>
+  </si>
+  <si>
+    <t>He1_4026A</t>
+  </si>
+  <si>
+    <t>4026.0</t>
+  </si>
+  <si>
+    <t>4026</t>
+  </si>
+  <si>
+    <t>4026A</t>
+  </si>
+  <si>
+    <t>$4026$ $HeI$</t>
+  </si>
+  <si>
+    <t>H1_4102A</t>
+  </si>
+  <si>
+    <t>4102.742</t>
+  </si>
+  <si>
+    <t>4102</t>
+  </si>
+  <si>
+    <t>4102A</t>
+  </si>
+  <si>
+    <t>$4102$ $H\delta$</t>
+  </si>
+  <si>
+    <t>H1_4341A</t>
+  </si>
+  <si>
+    <t>4341.471</t>
+  </si>
+  <si>
+    <t>4341</t>
+  </si>
+  <si>
+    <t>4341A</t>
+  </si>
+  <si>
+    <t>$4341$ $H\gamma$</t>
+  </si>
+  <si>
+    <t>O3_4363A</t>
+  </si>
+  <si>
+    <t>4363.21</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>4363</t>
+  </si>
+  <si>
+    <t>4363A</t>
+  </si>
+  <si>
+    <t>$4363$ $[OIII]$</t>
+  </si>
+  <si>
+    <t>He1_4471A</t>
+  </si>
+  <si>
+    <t>4471.0</t>
+  </si>
+  <si>
+    <t>4471</t>
+  </si>
+  <si>
+    <t>4471A</t>
+  </si>
+  <si>
+    <t>$4471$ $HeI$</t>
+  </si>
+  <si>
+    <t>Ar4_4740A</t>
+  </si>
+  <si>
+    <t>Ar4</t>
+  </si>
+  <si>
+    <t>4740A</t>
+  </si>
+  <si>
+    <t>$4470$ $[ArIV]$</t>
+  </si>
+  <si>
+    <t>He2_4686A</t>
+  </si>
+  <si>
+    <t>4686.0</t>
+  </si>
+  <si>
+    <t>He2r</t>
+  </si>
+  <si>
+    <t>4686A</t>
+  </si>
+  <si>
+    <t>$4686$ $HeII$</t>
+  </si>
+  <si>
+    <t>H1_4861A</t>
+  </si>
+  <si>
+    <t>4861.0</t>
+  </si>
+  <si>
+    <t>4861</t>
+  </si>
+  <si>
+    <t>4861A</t>
+  </si>
+  <si>
+    <t>$4861$ $H\beta$</t>
+  </si>
+  <si>
+    <t>O3_4959A</t>
+  </si>
+  <si>
+    <t>4958.911</t>
+  </si>
+  <si>
+    <t>4959</t>
+  </si>
+  <si>
+    <t>4959A</t>
+  </si>
+  <si>
+    <t>$4959$ $[OIII]$</t>
+  </si>
+  <si>
+    <t>O3_5007A</t>
+  </si>
+  <si>
+    <t>5006.843</t>
+  </si>
+  <si>
+    <t>5007</t>
+  </si>
+  <si>
+    <t>5007A</t>
+  </si>
+  <si>
+    <t>$5007$ $[OIII]$</t>
+  </si>
+  <si>
+    <t>N2_5755A</t>
+  </si>
+  <si>
+    <t>5755.0</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>5755</t>
+  </si>
+  <si>
+    <t>5755A</t>
+  </si>
+  <si>
+    <t>$5755$ $[NII]$</t>
+  </si>
+  <si>
+    <t>He1_5876A</t>
+  </si>
+  <si>
+    <t>5876.0</t>
+  </si>
+  <si>
+    <t>5876</t>
+  </si>
+  <si>
+    <t>5876A</t>
+  </si>
+  <si>
+    <t>$5876$ $HeI$</t>
+  </si>
+  <si>
+    <t>S3_6312A</t>
+  </si>
+  <si>
+    <t>6312.06</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>6312</t>
+  </si>
+  <si>
+    <t>6312A</t>
+  </si>
+  <si>
+    <t>$6312$ $[SIII]$</t>
+  </si>
+  <si>
+    <t>N2_6548A</t>
+  </si>
+  <si>
+    <t>6548.05</t>
+  </si>
+  <si>
+    <t>6548</t>
+  </si>
+  <si>
+    <t>6548A</t>
+  </si>
+  <si>
+    <t>$6548$ $[NII]$</t>
+  </si>
+  <si>
+    <t>H1_6563A</t>
+  </si>
+  <si>
+    <t>6562.819</t>
+  </si>
+  <si>
+    <t>6563</t>
+  </si>
+  <si>
+    <t>6563A</t>
+  </si>
+  <si>
+    <t>$6563$ $H\alpha$</t>
+  </si>
+  <si>
+    <t>N2_6584A</t>
+  </si>
+  <si>
+    <t>6583.46</t>
+  </si>
+  <si>
+    <t>6584</t>
+  </si>
+  <si>
+    <t>6584A</t>
+  </si>
+  <si>
+    <t>$6583$ $[NII]$</t>
+  </si>
+  <si>
+    <t>He1_6678A</t>
+  </si>
+  <si>
+    <t>6678.0</t>
+  </si>
+  <si>
+    <t>6678</t>
+  </si>
+  <si>
+    <t>6678A</t>
+  </si>
+  <si>
+    <t>$6678$ $HeI$</t>
+  </si>
+  <si>
+    <t>S2_6716A</t>
+  </si>
+  <si>
+    <t>6716.44</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>6716</t>
+  </si>
+  <si>
+    <t>6716A</t>
+  </si>
+  <si>
+    <t>$6717$ $[SII]$</t>
+  </si>
+  <si>
+    <t>S2_6731A</t>
+  </si>
+  <si>
+    <t>6730.81</t>
+  </si>
+  <si>
+    <t>6731</t>
+  </si>
+  <si>
+    <t>6731A</t>
+  </si>
+  <si>
+    <t>$6731$ $[SII]$</t>
+  </si>
+  <si>
+    <t>He1_7065A</t>
+  </si>
+  <si>
+    <t>7065.0</t>
+  </si>
+  <si>
+    <t>7065</t>
+  </si>
+  <si>
+    <t>7065A</t>
+  </si>
+  <si>
+    <t>$7065$ $HeI$</t>
+  </si>
+  <si>
+    <t>He1_7281A</t>
+  </si>
+  <si>
+    <t>7281.0</t>
+  </si>
+  <si>
+    <t>7281</t>
+  </si>
+  <si>
+    <t>7281A</t>
+  </si>
+  <si>
+    <t>$7281$ $HeI$</t>
+  </si>
+  <si>
+    <t>Ar3_7136A</t>
+  </si>
+  <si>
+    <t>Ar3</t>
+  </si>
+  <si>
+    <t>7136A</t>
+  </si>
+  <si>
+    <t>O2_7319A</t>
+  </si>
+  <si>
+    <t>7319.0</t>
+  </si>
+  <si>
+    <t>7319</t>
+  </si>
+  <si>
+    <t>7319A</t>
+  </si>
+  <si>
+    <t>$7319$ $[OII]$</t>
+  </si>
+  <si>
+    <t>7319A+</t>
+  </si>
+  <si>
+    <t>O2_7319A_b</t>
+  </si>
+  <si>
+    <t>7324.5</t>
+  </si>
+  <si>
+    <t>$7319 + 7330$ $[OII]$</t>
+  </si>
+  <si>
+    <t>O2_7330A</t>
+  </si>
+  <si>
+    <t>7330.0</t>
+  </si>
+  <si>
+    <t>7330</t>
+  </si>
+  <si>
+    <t>7330A</t>
+  </si>
+  <si>
+    <t>$7330$ $[OII]$</t>
+  </si>
+  <si>
+    <t>7330A+</t>
+  </si>
+  <si>
+    <t>Ar3_7751A</t>
+  </si>
+  <si>
+    <t>7751A</t>
+  </si>
+  <si>
+    <t>$7751$ $[NII]$</t>
+  </si>
+  <si>
+    <t>S3_9069A</t>
+  </si>
+  <si>
+    <t>9068.6</t>
+  </si>
+  <si>
+    <t>9069</t>
+  </si>
+  <si>
+    <t>9069A</t>
+  </si>
+  <si>
+    <t>$9069$ $[SIII]$</t>
+  </si>
+  <si>
+    <t>H1_9229A</t>
+  </si>
+  <si>
+    <t>9229.0</t>
+  </si>
+  <si>
+    <t>9229</t>
+  </si>
+  <si>
+    <t>9229A</t>
+  </si>
+  <si>
+    <t>$9229$ $Hpa9$</t>
+  </si>
+  <si>
+    <t>S3_9531A</t>
+  </si>
+  <si>
+    <t>9531.1</t>
+  </si>
+  <si>
+    <t>9531</t>
+  </si>
+  <si>
+    <t>9531A</t>
+  </si>
+  <si>
+    <t>$9531$ $[SIII]$</t>
+  </si>
+  <si>
+    <t>H1_9546A</t>
+  </si>
+  <si>
+    <t>9546.0</t>
+  </si>
+  <si>
+    <t>9546</t>
+  </si>
+  <si>
+    <t>9546A</t>
+  </si>
+  <si>
+    <t>$9531$ $Hpa9$</t>
+  </si>
+  <si>
+    <t>He1_10830A</t>
+  </si>
+  <si>
+    <t>10830.0</t>
+  </si>
+  <si>
+    <t>10830</t>
+  </si>
+  <si>
+    <t>10830A</t>
+  </si>
+  <si>
+    <t>$10830$ $HeI$</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>4102.0</t>
+  </si>
+  <si>
+    <t>4341.0</t>
+  </si>
+  <si>
+    <t>6563.0</t>
+  </si>
+  <si>
+    <t>He1</t>
+  </si>
+  <si>
+    <t>$7136$ $[ArIII]$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -670,35 +656,31 @@
       <family val="2"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="14"/>
       <color rgb="FF8DDAF8"/>
       <name val="Anonymous Pro"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <u val="single"/>
+      <i/>
+      <u/>
       <sz val="14"/>
       <color rgb="FF66AFF9"/>
       <name val="Anonymous Pro"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF66AFF9"/>
       <name val="Anonymous Pro"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="14"/>
       <color rgb="FF66AFF9"/>
       <name val="Anonymous Pro"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -711,7 +693,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -719,101 +701,53 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -872,36 +806,344 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="10.77"/>
+    <col min="1" max="1" width="26.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="10.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +1166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -947,7 +1189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -970,7 +1212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -984,7 +1226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1007,7 +1249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1030,7 +1272,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1053,7 +1295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1076,7 +1318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1122,7 +1364,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -1145,7 +1387,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -1168,7 +1410,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1191,17 +1433,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>4740</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>4740</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1214,7 +1456,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
@@ -1224,7 +1466,7 @@
       <c r="C15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>4686</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1237,7 +1479,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1260,7 +1502,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
@@ -1283,7 +1525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>86</v>
       </c>
@@ -1306,7 +1548,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1329,7 +1571,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
@@ -1352,7 +1594,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>102</v>
       </c>
@@ -1375,7 +1617,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>108</v>
       </c>
@@ -1398,7 +1640,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
@@ -1421,7 +1663,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>118</v>
       </c>
@@ -1444,7 +1686,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -1467,7 +1709,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
@@ -1490,7 +1732,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>134</v>
       </c>
@@ -1513,7 +1755,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>139</v>
       </c>
@@ -1536,7 +1778,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -1559,17 +1801,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="1">
         <v>7135.79</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="1">
         <v>7136</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1579,218 +1821,217 @@
         <v>19</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="H31" s="3" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>7751</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="1">
         <v>7751</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>195</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
@@ -1798,22 +2039,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.56"/>
+    <col min="1" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1831,7 +2069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1839,7 +2077,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>10</v>
@@ -1851,7 +2089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -1859,7 +2097,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>31</v>
@@ -1871,7 +2109,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
@@ -1879,7 +2117,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>38</v>
@@ -1891,15 +2129,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>48</v>
@@ -1911,15 +2149,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>53</v>
@@ -1931,7 +2169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1939,7 +2177,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>78</v>
@@ -1951,15 +2189,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>115</v>
@@ -1971,47 +2209,47 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>189</v>
-      </c>
       <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
@@ -2019,7 +2257,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
@@ -2027,7 +2265,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>31</v>
@@ -2039,7 +2277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
@@ -2047,7 +2285,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>43</v>
@@ -2059,7 +2297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>62</v>
       </c>
@@ -2067,7 +2305,7 @@
         <v>63</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>64</v>
@@ -2079,7 +2317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>97</v>
       </c>
@@ -2087,7 +2325,7 @@
         <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>99</v>
@@ -2099,7 +2337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>123</v>
       </c>
@@ -2107,7 +2345,7 @@
         <v>124</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>125</v>
@@ -2119,7 +2357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>139</v>
       </c>
@@ -2127,7 +2365,7 @@
         <v>140</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>141</v>
@@ -2139,7 +2377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>144</v>
       </c>
@@ -2147,7 +2385,7 @@
         <v>145</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>146</v>
@@ -2159,27 +2397,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>194</v>
-      </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
@@ -2187,7 +2425,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>128</v>
       </c>
@@ -2207,7 +2445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>134</v>
       </c>
@@ -2227,7 +2465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="4"/>
@@ -2235,7 +2473,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>102</v>
       </c>
@@ -2255,47 +2493,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="F25" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="F26" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
@@ -2303,7 +2541,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
@@ -2343,47 +2581,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>156</v>
-      </c>
       <c r="F30" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="F31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
@@ -2391,7 +2629,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>56</v>
       </c>
@@ -2411,7 +2649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>81</v>
       </c>
@@ -2431,7 +2669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>86</v>
       </c>
@@ -2451,7 +2689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="4"/>
@@ -2459,7 +2697,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>91</v>
       </c>
@@ -2479,7 +2717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>108</v>
       </c>
@@ -2499,7 +2737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>118</v>
       </c>
@@ -2519,7 +2757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4"/>
@@ -2527,17 +2765,17 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="4" t="n">
+      <c r="B41" s="4">
         <v>7135.79</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="4" t="n">
+      <c r="D41" s="4">
         <v>7136</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -2547,37 +2785,37 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B42" s="4" t="n">
+        <v>167</v>
+      </c>
+      <c r="B42" s="4">
         <v>7751</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D42" s="4">
         <v>7751</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="4">
         <v>4740</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="4">
         <v>4740</v>
       </c>
       <c r="E43" s="11" t="s">
@@ -2588,10 +2826,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>